<commit_message>
new analysis with revised BKT model
</commit_message>
<xml_diff>
--- a/Data/Result_Step.xlsx
+++ b/Data/Result_Step.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project\AL\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C16BCFC-41DA-414B-92E4-1F97419E91CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A3F711F-89E4-43C2-9C3E-64972EB035E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28956" yWindow="792" windowWidth="14568" windowHeight="12276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20676" yWindow="876" windowWidth="16596" windowHeight="12276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Rollup_Log" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="BKTparameters" sheetId="1" r:id="rId1"/>
+    <sheet name="count" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="57">
   <si>
     <t>Opportunity (ptype_selection)</t>
   </si>
@@ -113,16 +113,109 @@
   </si>
   <si>
     <t>M done</t>
+  </si>
+  <si>
+    <t>intercept</t>
+  </si>
+  <si>
+    <t>slope</t>
+  </si>
+  <si>
+    <t>guess</t>
+  </si>
+  <si>
+    <t>slip</t>
+  </si>
+  <si>
+    <t>M  JCommTable6.R0C0</t>
+  </si>
+  <si>
+    <t>M  JCommTable6.R1C0</t>
+  </si>
+  <si>
+    <t>M  done</t>
+  </si>
+  <si>
+    <t>AD JCommTable6.R0C0</t>
+  </si>
+  <si>
+    <t>AD JCommTable6.R1C0</t>
+  </si>
+  <si>
+    <t>AD done</t>
+  </si>
+  <si>
+    <t>AD JCommTable8.R0C0</t>
+  </si>
+  <si>
+    <t>AD JCommTable4.R1C0</t>
+  </si>
+  <si>
+    <t>AD JCommTable4.R0C0</t>
+  </si>
+  <si>
+    <t>AD JCommTable5.R1C0</t>
+  </si>
+  <si>
+    <t>AD JCommTable5.R0C0</t>
+  </si>
+  <si>
+    <t>M  JCommTable8.R0C0</t>
+  </si>
+  <si>
+    <t>M  JCommTable4.R1C0</t>
+  </si>
+  <si>
+    <t>AS JCommTable8.R0C0</t>
+  </si>
+  <si>
+    <t>AS JCommTable6.R1C0</t>
+  </si>
+  <si>
+    <t>AS JCommTable6.R0C0</t>
+  </si>
+  <si>
+    <t>AS done</t>
+  </si>
+  <si>
+    <t>M  JCommTable4.R0C0</t>
+  </si>
+  <si>
+    <t>M  JCommTable5.R1C0</t>
+  </si>
+  <si>
+    <t>AS JCommTable4.R0C0</t>
+  </si>
+  <si>
+    <t>AS JCommTable4.R1C0</t>
+  </si>
+  <si>
+    <t>AS JCommTable5.R0C0</t>
+  </si>
+  <si>
+    <t>AS JCommTable5.R1C0</t>
+  </si>
+  <si>
+    <t>M  JCommTable5.R0C0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000000000"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -154,13 +247,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,23 +537,458 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="12.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0.1664681482</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0.45031236559999999</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0.17169945649999999</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1.17767E-5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1.6265410000000001E-4</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.26859084989999998</v>
+      </c>
+      <c r="D3" s="4">
+        <v>4.3543950200000001E-2</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0.1206098664</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="4">
+        <v>6.6122100000000003E-4</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.33789189819999998</v>
+      </c>
+      <c r="D4" s="4">
+        <v>7.0383388099999999E-2</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.1035722555</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1.2292259999999999E-4</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.23149003360000001</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1.5138728400000001E-2</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0.2526931</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="4">
+        <v>2.7418899999999999E-5</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.24509906540000001</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.13279621680000001</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.13170298629999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="4">
+        <v>2.3957000000000002E-6</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.1507513606</v>
+      </c>
+      <c r="D7" s="4">
+        <v>9.3103508000000005E-3</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0.26151002639999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="4">
+        <v>6.0205199999999997E-5</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.1446901951</v>
+      </c>
+      <c r="D8" s="4">
+        <v>4.5431496100000003E-2</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="4">
+        <v>7.1258999999999998E-6</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.53359764099999996</v>
+      </c>
+      <c r="D9" s="4">
+        <v>5.5097333499999998E-2</v>
+      </c>
+      <c r="E9" s="4">
+        <v>5.3556306099999999E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0.25392906910000002</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.47817773050000001</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="E10" s="4">
+        <v>6.4905379999999997E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="4">
+        <v>0.36566256860000002</v>
+      </c>
+      <c r="C11" s="4">
+        <v>1.0960538000000001E-3</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="4">
+        <v>0.35535588800000001</v>
+      </c>
+      <c r="C12" s="4">
+        <v>9.5224950000000002E-4</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="4">
+        <v>0.22925549179999999</v>
+      </c>
+      <c r="C13" s="4">
+        <v>1.6173798E-3</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0</v>
+      </c>
+      <c r="E13" s="4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="C14" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D14" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="E14" s="4">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="4">
+        <v>4.862E-7</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0.29957131259999997</v>
+      </c>
+      <c r="D15" s="4">
+        <v>8.9968288899999999E-2</v>
+      </c>
+      <c r="E15" s="4">
+        <v>5.0038190000000003E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="4">
+        <v>1.3000000000000001E-9</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0.32414618680000001</v>
+      </c>
+      <c r="D16" s="4">
+        <v>8.6730740099999995E-2</v>
+      </c>
+      <c r="E16" s="4">
+        <v>4.3733013699999997E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="4">
+        <v>0.1078957988</v>
+      </c>
+      <c r="C17" s="4">
+        <v>1.0825429E-3</v>
+      </c>
+      <c r="D17" s="4">
+        <v>0</v>
+      </c>
+      <c r="E17" s="4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="4">
+        <v>4.5219100000000002E-5</v>
+      </c>
+      <c r="C18" s="4">
+        <v>0.41356532579999999</v>
+      </c>
+      <c r="D18" s="4">
+        <v>0.1296995406</v>
+      </c>
+      <c r="E18" s="4">
+        <v>8.6936491000000008E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="4">
+        <v>0.2810030275</v>
+      </c>
+      <c r="C19" s="4">
+        <v>1.0226739999999999E-3</v>
+      </c>
+      <c r="D19" s="4">
+        <v>0</v>
+      </c>
+      <c r="E19" s="4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="4">
+        <v>0.16397737000000001</v>
+      </c>
+      <c r="C20" s="4">
+        <v>1.5620670000000001E-4</v>
+      </c>
+      <c r="D20" s="4">
+        <v>0</v>
+      </c>
+      <c r="E20" s="4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="4">
+        <v>0.38858173509999999</v>
+      </c>
+      <c r="C21" s="4">
+        <v>1.6173798E-3</v>
+      </c>
+      <c r="D21" s="4">
+        <v>0</v>
+      </c>
+      <c r="E21" s="4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="4">
+        <v>0.14056931819999999</v>
+      </c>
+      <c r="C22" s="4">
+        <v>3.2399220000000001E-4</v>
+      </c>
+      <c r="D22" s="4">
+        <v>0</v>
+      </c>
+      <c r="E22" s="4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="4">
+        <v>1.04595E-5</v>
+      </c>
+      <c r="C23" s="4">
+        <v>0.25507604150000002</v>
+      </c>
+      <c r="D23" s="4">
+        <v>0.1236774948</v>
+      </c>
+      <c r="E23" s="4">
+        <v>4.5628232800000001E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="4">
+        <v>1.1154835E-3</v>
+      </c>
+      <c r="C24" s="4">
+        <v>0.33868264450000002</v>
+      </c>
+      <c r="D24" s="4">
+        <v>0.1267294561</v>
+      </c>
+      <c r="E24" s="4">
+        <v>3.9674046099999999E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="4">
+        <v>0.18565179700000001</v>
+      </c>
+      <c r="C25" s="4">
+        <v>1.6173798E-3</v>
+      </c>
+      <c r="D25" s="4">
+        <v>0</v>
+      </c>
+      <c r="E25" s="4">
+        <v>0.3</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E25">
+    <sortCondition ref="A1:A25"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD62F0AE-7533-4854-AD8C-44590DB3ACB3}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
@@ -468,14 +998,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2"/>
+      <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -563,13 +1093,13 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B7">
         <v>10.766667</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>30</v>
       </c>
       <c r="D7" s="1">
@@ -580,13 +1110,13 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B8">
         <v>10.566667000000001</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>30</v>
       </c>
       <c r="D8" s="1">
@@ -699,13 +1229,13 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B15">
         <v>4.5333329999999998</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="2">
         <v>30</v>
       </c>
       <c r="D15" s="1">
@@ -716,13 +1246,13 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B16">
         <v>4.0333329999999998</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="2">
         <v>30</v>
       </c>
       <c r="D16" s="1">
@@ -835,13 +1365,13 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B23">
         <v>16.100000000000001</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="2">
         <v>30</v>
       </c>
       <c r="D23" s="1">
@@ -852,13 +1382,13 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B24">
         <v>16.333333</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="2">
         <v>30</v>
       </c>
       <c r="D24" s="1">

</xml_diff>